<commit_message>
updated and added new templates
</commit_message>
<xml_diff>
--- a/ISRaD_data_files/Houston_2024.xlsx
+++ b/ISRaD_data_files/Houston_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f0076db\Documents\GitHub\ISRaD\ISRaD_data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08836CDE-F086-4816-B36F-BB3301AF9736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D703C52-5253-4BD4-8573-D06153149D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4102,9 +4102,6 @@
     <t>Houston, A., Garnett, M.H., Austin, W.E.N., 2024, Blue carbon additionality: New insights from the radiocarbon content of saltmarsh soils and their respired CO2, Limnology and Oceanography, 69, 548-561.</t>
   </si>
   <si>
-    <t>saltmarsh soil incubations</t>
-  </si>
-  <si>
     <t>Kyle of Tongue</t>
   </si>
   <si>
@@ -4370,6 +4367,9 @@
   </si>
   <si>
     <t>freeze dried to a constant mass</t>
+  </si>
+  <si>
+    <t>saltmarsh soil incubations; respired CO2 data received directly from authors</t>
   </si>
 </sst>
 </file>
@@ -6578,8 +6578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q985"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -6784,7 +6784,7 @@
         <v>996</v>
       </c>
       <c r="N4" s="126" t="s">
-        <v>997</v>
+        <v>1086</v>
       </c>
       <c r="O4" s="124"/>
       <c r="P4" s="140">
@@ -7907,7 +7907,7 @@
         <v>989</v>
       </c>
       <c r="B4" s="127" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C4">
         <v>58.447189000000002</v>
@@ -7924,7 +7924,7 @@
         <v>989</v>
       </c>
       <c r="B5" s="127" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C5" s="127">
         <v>56.566968000000003</v>
@@ -7941,7 +7941,7 @@
         <v>989</v>
       </c>
       <c r="B6" s="127" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C6" s="127">
         <v>56.058194999999998</v>
@@ -9640,11 +9640,11 @@
         <v>989</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -9688,11 +9688,11 @@
         <v>989</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
@@ -9736,11 +9736,11 @@
         <v>989</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
@@ -9784,11 +9784,11 @@
         <v>989</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -9832,11 +9832,11 @@
         <v>989</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
@@ -9880,11 +9880,11 @@
         <v>989</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
@@ -9928,10 +9928,10 @@
         <v>989</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>999</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>1000</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>1001</v>
       </c>
       <c r="E10" s="3"/>
       <c r="I10" s="12" t="s">
@@ -9950,10 +9950,10 @@
         <v>989</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E11" s="3"/>
       <c r="I11" s="12" t="s">
@@ -9972,10 +9972,10 @@
         <v>989</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E12" s="3"/>
       <c r="I12" s="12" t="s">
@@ -19295,13 +19295,13 @@
         <v>989</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="E4" s="113">
         <v>2022</v>
@@ -19330,7 +19330,7 @@
         <v>0.23</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
@@ -19375,7 +19375,7 @@
         <v>-27.3</v>
       </c>
       <c r="BD4" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BE4" s="5"/>
       <c r="BF4" s="5"/>
@@ -19444,13 +19444,13 @@
         <v>989</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="E5" s="113">
         <v>2022</v>
@@ -19479,7 +19479,7 @@
         <v>0.44</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
@@ -19524,7 +19524,7 @@
         <v>-27.6</v>
       </c>
       <c r="BD5" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BE5" s="5"/>
       <c r="BF5" s="5"/>
@@ -19593,13 +19593,13 @@
         <v>989</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="E6" s="113">
         <v>2022</v>
@@ -19628,7 +19628,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
@@ -19673,7 +19673,7 @@
         <v>-26.7</v>
       </c>
       <c r="BD6" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BE6" s="5"/>
       <c r="BF6" s="5"/>
@@ -19742,13 +19742,13 @@
         <v>989</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="E7" s="113">
         <v>2022</v>
@@ -19777,7 +19777,7 @@
         <v>0.44</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
@@ -19822,7 +19822,7 @@
         <v>-24.2</v>
       </c>
       <c r="BD7" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BE7" s="5"/>
       <c r="BF7" s="5"/>
@@ -19891,13 +19891,13 @@
         <v>989</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E8" s="113">
         <v>2022</v>
@@ -19926,7 +19926,7 @@
         <v>0.8</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
@@ -19971,7 +19971,7 @@
         <v>-26.4</v>
       </c>
       <c r="BD8" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BE8" s="5"/>
       <c r="BF8" s="5"/>
@@ -20040,13 +20040,13 @@
         <v>989</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="E9" s="113">
         <v>2022</v>
@@ -20064,7 +20064,7 @@
         <v>0.47</v>
       </c>
       <c r="U9" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB9" s="5"/>
       <c r="AR9" s="179">
@@ -20080,7 +20080,7 @@
         <v>-25.6</v>
       </c>
       <c r="BD9" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ9" s="3">
         <v>0.90110000000000001</v>
@@ -20094,13 +20094,13 @@
         <v>989</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="E10" s="113">
         <v>2022</v>
@@ -20118,7 +20118,7 @@
         <v>0.47</v>
       </c>
       <c r="U10" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB10" s="5"/>
       <c r="AR10" s="179">
@@ -20134,7 +20134,7 @@
         <v>-26.3</v>
       </c>
       <c r="BD10" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ10" s="3">
         <v>0.95289999999999997</v>
@@ -20148,13 +20148,13 @@
         <v>989</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="E11" s="113">
         <v>2022</v>
@@ -20172,7 +20172,7 @@
         <v>0.43</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB11" s="5"/>
       <c r="AR11" s="179">
@@ -20188,7 +20188,7 @@
         <v>-24.8</v>
       </c>
       <c r="BD11" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ11" s="3">
         <v>0.98219999999999996</v>
@@ -20202,13 +20202,13 @@
         <v>989</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E12" s="113">
         <v>2022</v>
@@ -20226,7 +20226,7 @@
         <v>0.92</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB12" s="5"/>
       <c r="AR12" s="179">
@@ -20242,7 +20242,7 @@
         <v>-26</v>
       </c>
       <c r="BD12" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ12" s="3">
         <v>1.0685</v>
@@ -20256,13 +20256,13 @@
         <v>989</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E13" s="113">
         <v>2022</v>
@@ -20280,7 +20280,7 @@
         <v>0.47</v>
       </c>
       <c r="U13" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB13" s="5"/>
       <c r="AR13" s="179">
@@ -20296,7 +20296,7 @@
         <v>-26.2</v>
       </c>
       <c r="BD13" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ13" s="3">
         <v>0.96640000000000004</v>
@@ -20310,13 +20310,13 @@
         <v>989</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="E14" s="113">
         <v>2022</v>
@@ -20334,7 +20334,7 @@
         <v>0.24</v>
       </c>
       <c r="U14" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB14" s="5"/>
       <c r="AR14" s="179">
@@ -20350,7 +20350,7 @@
         <v>-26.6</v>
       </c>
       <c r="BD14" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ14" s="3">
         <v>1.0482</v>
@@ -20364,13 +20364,13 @@
         <v>989</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E15" s="113">
         <v>2022</v>
@@ -20388,7 +20388,7 @@
         <v>0.5</v>
       </c>
       <c r="U15" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB15" s="5"/>
       <c r="AR15" s="179">
@@ -20404,7 +20404,7 @@
         <v>-24.6</v>
       </c>
       <c r="BD15" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ15" s="3">
         <v>0.66739999999999999</v>
@@ -20418,13 +20418,13 @@
         <v>989</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="E16" s="113">
         <v>2022</v>
@@ -20442,7 +20442,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="U16" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB16" s="5"/>
       <c r="AR16" s="179">
@@ -20458,7 +20458,7 @@
         <v>-26.4</v>
       </c>
       <c r="BD16" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ16" s="3">
         <v>0.99680000000000002</v>
@@ -20472,13 +20472,13 @@
         <v>989</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="E17" s="113">
         <v>2022</v>
@@ -20496,7 +20496,7 @@
         <v>0.5</v>
       </c>
       <c r="U17" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB17" s="5"/>
       <c r="AR17" s="179">
@@ -20512,7 +20512,7 @@
         <v>-26</v>
       </c>
       <c r="BD17" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ17" s="3">
         <v>1.0105</v>
@@ -20526,13 +20526,13 @@
         <v>989</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="E18" s="113">
         <v>2022</v>
@@ -20550,7 +20550,7 @@
         <v>0.67</v>
       </c>
       <c r="U18" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB18" s="5"/>
       <c r="AR18" s="179">
@@ -20566,7 +20566,7 @@
         <v>-25.8</v>
       </c>
       <c r="BD18" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ18" s="3">
         <v>1.0196000000000001</v>
@@ -20580,13 +20580,13 @@
         <v>989</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="E19" s="113">
         <v>2022</v>
@@ -20604,7 +20604,7 @@
         <v>0.44</v>
       </c>
       <c r="U19" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB19" s="5"/>
       <c r="AR19" s="179">
@@ -20620,7 +20620,7 @@
         <v>-23.4</v>
       </c>
       <c r="BD19" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ19" s="3">
         <v>0.98960000000000004</v>
@@ -20634,13 +20634,13 @@
         <v>989</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="E20" s="113">
         <v>2022</v>
@@ -20658,7 +20658,7 @@
         <v>0.39</v>
       </c>
       <c r="U20" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB20" s="5"/>
       <c r="AR20" s="179">
@@ -20674,7 +20674,7 @@
         <v>-26.7</v>
       </c>
       <c r="BD20" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ20" s="3">
         <v>1.1202000000000001</v>
@@ -20688,13 +20688,13 @@
         <v>989</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="E21" s="113">
         <v>2022</v>
@@ -20712,7 +20712,7 @@
         <v>0.26</v>
       </c>
       <c r="U21" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB21" s="5"/>
       <c r="AR21" s="179">
@@ -20728,7 +20728,7 @@
         <v>-25.3</v>
       </c>
       <c r="BD21" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ21" s="3">
         <v>0.98219999999999996</v>
@@ -20742,13 +20742,13 @@
         <v>989</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>999</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>1000</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>1001</v>
-      </c>
       <c r="D22" s="9" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="E22" s="113">
         <v>2022</v>
@@ -20766,7 +20766,7 @@
         <v>0.45</v>
       </c>
       <c r="U22" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB22" s="5"/>
       <c r="AR22" s="179">
@@ -20782,7 +20782,7 @@
         <v>-23.5</v>
       </c>
       <c r="BD22" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ22" s="3">
         <v>0.47489999999999999</v>
@@ -20796,13 +20796,13 @@
         <v>989</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>999</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>1000</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>1001</v>
-      </c>
       <c r="D23" s="9" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="E23" s="113">
         <v>2022</v>
@@ -20820,7 +20820,7 @@
         <v>0.37</v>
       </c>
       <c r="U23" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB23" s="5"/>
       <c r="AR23" s="179">
@@ -20836,7 +20836,7 @@
         <v>-24.5</v>
       </c>
       <c r="BD23" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ23" s="3">
         <v>0.45029999999999998</v>
@@ -20850,13 +20850,13 @@
         <v>989</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>999</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>1000</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>1001</v>
-      </c>
       <c r="D24" s="9" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="E24" s="113">
         <v>2022</v>
@@ -20874,7 +20874,7 @@
         <v>0.33</v>
       </c>
       <c r="U24" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB24" s="5"/>
       <c r="AR24" s="179">
@@ -20890,7 +20890,7 @@
         <v>-23.8</v>
       </c>
       <c r="BD24" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ24" s="3">
         <v>0.41360000000000002</v>
@@ -20904,13 +20904,13 @@
         <v>989</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="E25" s="113">
         <v>2022</v>
@@ -20928,7 +20928,7 @@
         <v>0.39</v>
       </c>
       <c r="U25" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB25" s="5"/>
       <c r="AR25" s="179">
@@ -20944,7 +20944,7 @@
         <v>-22.2</v>
       </c>
       <c r="BD25" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ25" s="3">
         <v>0.31469999999999998</v>
@@ -20958,13 +20958,13 @@
         <v>989</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="E26" s="113">
         <v>2022</v>
@@ -20982,7 +20982,7 @@
         <v>0.53</v>
       </c>
       <c r="U26" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB26" s="5"/>
       <c r="AR26" s="179">
@@ -20998,7 +20998,7 @@
         <v>-24.1</v>
       </c>
       <c r="BD26" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ26" s="3">
         <v>0.43690000000000001</v>
@@ -21012,13 +21012,13 @@
         <v>989</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="E27" s="113">
         <v>2022</v>
@@ -21036,7 +21036,7 @@
         <v>0.19</v>
       </c>
       <c r="U27" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB27" s="5"/>
       <c r="AR27" s="179">
@@ -21052,7 +21052,7 @@
         <v>-25.1</v>
       </c>
       <c r="BD27" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ27" s="3">
         <v>0.50929999999999997</v>
@@ -21066,13 +21066,13 @@
         <v>989</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="E28" s="113">
         <v>2022</v>
@@ -21090,7 +21090,7 @@
         <v>0.35</v>
       </c>
       <c r="U28" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB28" s="5"/>
       <c r="AR28" s="179">
@@ -21106,7 +21106,7 @@
         <v>-23.7</v>
       </c>
       <c r="BD28" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ28" s="3">
         <v>0.4703</v>
@@ -21120,13 +21120,13 @@
         <v>989</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="E29" s="113">
         <v>2022</v>
@@ -21144,7 +21144,7 @@
         <v>0.51</v>
       </c>
       <c r="U29" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB29" s="5"/>
       <c r="AR29" s="179">
@@ -21160,7 +21160,7 @@
         <v>-24</v>
       </c>
       <c r="BD29" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ29" s="3">
         <v>0.4415</v>
@@ -21174,13 +21174,13 @@
         <v>989</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="E30" s="113">
         <v>2022</v>
@@ -21198,7 +21198,7 @@
         <v>0.38</v>
       </c>
       <c r="U30" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="AB30" s="5"/>
       <c r="AR30" s="180">
@@ -21214,7 +21214,7 @@
         <v>-24.1</v>
       </c>
       <c r="BD30" s="181" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="BJ30" s="3">
         <v>0.44479999999999997</v>
@@ -29474,16 +29474,16 @@
         <v>989</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="F4" s="181" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>725</v>
@@ -29510,7 +29510,7 @@
         <v>-28.3</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE4" s="3">
         <v>1.0057</v>
@@ -29524,16 +29524,16 @@
         <v>989</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="F5" s="181" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>725</v>
@@ -29560,7 +29560,7 @@
         <v>-25</v>
       </c>
       <c r="Y5" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE5" s="3">
         <v>1.0103</v>
@@ -29574,16 +29574,16 @@
         <v>989</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="F6" s="181" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>725</v>
@@ -29610,7 +29610,7 @@
         <v>-24.3</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE6" s="3">
         <v>0.94889999999999997</v>
@@ -29624,16 +29624,16 @@
         <v>989</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="F7" s="181" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>725</v>
@@ -29660,7 +29660,7 @@
         <v>-27.7</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE7" s="3">
         <v>0.99729999999999996</v>
@@ -29674,16 +29674,16 @@
         <v>989</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="F8" s="181" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>725</v>
@@ -29710,7 +29710,7 @@
         <v>-27.9</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE8" s="3">
         <v>1.0206999999999999</v>
@@ -29724,16 +29724,16 @@
         <v>989</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="F9" s="181" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>725</v>
@@ -29760,7 +29760,7 @@
         <v>-25.4</v>
       </c>
       <c r="Y9" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE9" s="3">
         <v>1.0423</v>
@@ -29774,16 +29774,16 @@
         <v>989</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F10" s="181" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>725</v>
@@ -29810,7 +29810,7 @@
         <v>-28.7</v>
       </c>
       <c r="Y10" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE10" s="3">
         <v>1.0203</v>
@@ -29824,16 +29824,16 @@
         <v>989</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F11" s="181" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>725</v>
@@ -29860,7 +29860,7 @@
         <v>-27.3</v>
       </c>
       <c r="Y11" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE11" s="3">
         <v>1.0201</v>
@@ -29874,16 +29874,16 @@
         <v>989</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="F12" s="181" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>725</v>
@@ -29910,7 +29910,7 @@
         <v>-22.7</v>
       </c>
       <c r="Y12" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE12" s="3">
         <v>1.0097</v>
@@ -29924,16 +29924,16 @@
         <v>989</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="F13" s="181" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>725</v>
@@ -29960,7 +29960,7 @@
         <v>-24.6</v>
       </c>
       <c r="Y13" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE13" s="3">
         <v>1.0065999999999999</v>
@@ -29974,16 +29974,16 @@
         <v>989</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="F14" s="181" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>725</v>
@@ -30010,7 +30010,7 @@
         <v>-27</v>
       </c>
       <c r="Y14" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE14" s="3">
         <v>1.0625</v>
@@ -30024,16 +30024,16 @@
         <v>989</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="F15" s="181" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>725</v>
@@ -30060,7 +30060,7 @@
         <v>-23.1</v>
       </c>
       <c r="Y15" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE15" s="3">
         <v>1.2012</v>
@@ -30074,16 +30074,16 @@
         <v>989</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="F16" s="181" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>725</v>
@@ -30110,7 +30110,7 @@
         <v>-24.9</v>
       </c>
       <c r="Y16" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE16" s="3">
         <v>1.0175000000000001</v>
@@ -30124,16 +30124,16 @@
         <v>989</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="F17" s="181" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>725</v>
@@ -30160,7 +30160,7 @@
         <v>-24.2</v>
       </c>
       <c r="Y17" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE17" s="3">
         <v>1.0434000000000001</v>
@@ -30174,16 +30174,16 @@
         <v>989</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="F18" s="181" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>725</v>
@@ -30210,7 +30210,7 @@
         <v>-21.1</v>
       </c>
       <c r="Y18" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE18" s="3">
         <v>1.0658000000000001</v>
@@ -30224,16 +30224,16 @@
         <v>989</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="F19" s="181" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>725</v>
@@ -30260,7 +30260,7 @@
         <v>-26.8</v>
       </c>
       <c r="Y19" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE19" s="3">
         <v>1.0258</v>
@@ -30274,16 +30274,16 @@
         <v>989</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="F20" s="181" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>725</v>
@@ -30310,7 +30310,7 @@
         <v>-26.1</v>
       </c>
       <c r="Y20" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE20" s="3">
         <v>1.0384</v>
@@ -30324,16 +30324,16 @@
         <v>989</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="F21" s="181" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>725</v>
@@ -30360,7 +30360,7 @@
         <v>-25</v>
       </c>
       <c r="Y21" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE21" s="3">
         <v>1.0253000000000001</v>
@@ -30374,16 +30374,16 @@
         <v>989</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>999</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>1000</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>1001</v>
-      </c>
       <c r="D22" s="9" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="F22" s="181" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>725</v>
@@ -30410,7 +30410,7 @@
         <v>-23.3</v>
       </c>
       <c r="Y22" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE22" s="3">
         <v>0.99150000000000005</v>
@@ -30424,16 +30424,16 @@
         <v>989</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>999</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>1000</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>1001</v>
-      </c>
       <c r="D23" s="9" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F23" s="181" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>725</v>
@@ -30460,7 +30460,7 @@
         <v>-23.6</v>
       </c>
       <c r="Y23" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE23" s="3">
         <v>0.87180000000000002</v>
@@ -30474,16 +30474,16 @@
         <v>989</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>999</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>1000</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>1001</v>
-      </c>
       <c r="D24" s="9" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F24" s="181" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>725</v>
@@ -30510,7 +30510,7 @@
         <v>-6.1</v>
       </c>
       <c r="Y24" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE24" s="3">
         <v>0.36130000000000001</v>
@@ -30524,16 +30524,16 @@
         <v>989</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="F25" s="181" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>725</v>
@@ -30560,7 +30560,7 @@
         <v>-22.9</v>
       </c>
       <c r="Y25" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE25" s="3">
         <v>0.98970000000000002</v>
@@ -30574,16 +30574,16 @@
         <v>989</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="F26" s="181" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>725</v>
@@ -30610,7 +30610,7 @@
         <v>-23.1</v>
       </c>
       <c r="Y26" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE26" s="3">
         <v>0.90259999999999996</v>
@@ -30624,16 +30624,16 @@
         <v>989</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="F27" s="181" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>725</v>
@@ -30660,7 +30660,7 @@
         <v>-20.2</v>
       </c>
       <c r="Y27" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE27" s="3">
         <v>0.94850000000000001</v>
@@ -30674,16 +30674,16 @@
         <v>989</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="F28" s="181" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>725</v>
@@ -30710,7 +30710,7 @@
         <v>-20.6</v>
       </c>
       <c r="Y28" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE28" s="3">
         <v>0.97560000000000002</v>
@@ -30724,16 +30724,16 @@
         <v>989</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="F29" s="181" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>725</v>
@@ -30760,7 +30760,7 @@
         <v>-23.4</v>
       </c>
       <c r="Y29" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE29" s="3">
         <v>0.88219999999999998</v>
@@ -30774,16 +30774,16 @@
         <v>989</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="F30" s="181" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>725</v>
@@ -30810,7 +30810,7 @@
         <v>-3.7</v>
       </c>
       <c r="Y30" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE30" s="3">
         <v>0.28249999999999997</v>
@@ -30824,16 +30824,16 @@
         <v>989</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="F31" s="181" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>725</v>
@@ -30863,16 +30863,16 @@
         <v>989</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="F32" s="181" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>725</v>
@@ -30899,7 +30899,7 @@
         <v>-28.7</v>
       </c>
       <c r="Y32" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE32" s="3">
         <v>1.0026999999999999</v>
@@ -30913,16 +30913,16 @@
         <v>989</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="F33" s="181" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>725</v>
@@ -30952,16 +30952,16 @@
         <v>989</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="F34" s="181" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>725</v>
@@ -30991,16 +30991,16 @@
         <v>989</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="F35" s="181" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>725</v>
@@ -31027,7 +31027,7 @@
         <v>-29.1</v>
       </c>
       <c r="Y35" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE35" s="3">
         <v>1.0007999999999999</v>
@@ -31041,16 +31041,16 @@
         <v>989</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="F36" s="181" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>725</v>
@@ -31080,16 +31080,16 @@
         <v>989</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F37" s="181" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>725</v>
@@ -31119,16 +31119,16 @@
         <v>989</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F38" s="181" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>725</v>
@@ -31155,7 +31155,7 @@
         <v>-28.2</v>
       </c>
       <c r="Y38" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE38" s="3">
         <v>1.0088999999999999</v>
@@ -31169,16 +31169,16 @@
         <v>989</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="F39" s="181" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>725</v>
@@ -31208,16 +31208,16 @@
         <v>989</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="F40" s="181" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>725</v>
@@ -31247,16 +31247,16 @@
         <v>989</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="F41" s="181" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>725</v>
@@ -31283,7 +31283,7 @@
         <v>-26.9</v>
       </c>
       <c r="Y41" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE41" s="3">
         <v>1.0754999999999999</v>
@@ -31297,16 +31297,16 @@
         <v>989</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="F42" s="181" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>725</v>
@@ -31336,16 +31336,16 @@
         <v>989</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="F43" s="181" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>725</v>
@@ -31375,16 +31375,16 @@
         <v>989</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="F44" s="181" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>725</v>
@@ -31411,7 +31411,7 @@
         <v>-27.3</v>
       </c>
       <c r="Y44" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE44" s="3">
         <v>1.0384</v>
@@ -31425,16 +31425,16 @@
         <v>989</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="F45" s="181" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>725</v>
@@ -31464,16 +31464,16 @@
         <v>989</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="F46" s="181" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>725</v>
@@ -31503,16 +31503,16 @@
         <v>989</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="F47" s="181" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>725</v>
@@ -31539,7 +31539,7 @@
         <v>-26.6</v>
       </c>
       <c r="Y47" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE47" s="3">
         <v>1.0450999999999999</v>
@@ -31553,16 +31553,16 @@
         <v>989</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="F48" s="181" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>725</v>
@@ -31592,16 +31592,16 @@
         <v>989</v>
       </c>
       <c r="B49" s="9" t="s">
+        <v>999</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>1000</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>1001</v>
-      </c>
       <c r="D49" s="9" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="F49" s="181" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>725</v>
@@ -31631,16 +31631,16 @@
         <v>989</v>
       </c>
       <c r="B50" s="9" t="s">
+        <v>999</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>1000</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>1001</v>
-      </c>
       <c r="D50" s="9" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F50" s="181" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>725</v>
@@ -31667,7 +31667,7 @@
         <v>-23.9</v>
       </c>
       <c r="Y50" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE50" s="3">
         <v>0.84099999999999997</v>
@@ -31681,16 +31681,16 @@
         <v>989</v>
       </c>
       <c r="B51" s="9" t="s">
+        <v>999</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>1000</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>1001</v>
-      </c>
       <c r="D51" s="9" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F51" s="181" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>725</v>
@@ -31720,16 +31720,16 @@
         <v>989</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="F52" s="181" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>725</v>
@@ -31759,16 +31759,16 @@
         <v>989</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="F53" s="181" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>725</v>
@@ -31795,7 +31795,7 @@
         <v>-17.899999999999999</v>
       </c>
       <c r="Y53" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE53" s="3">
         <v>0.67689999999999995</v>
@@ -31809,16 +31809,16 @@
         <v>989</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="F54" s="181" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>725</v>
@@ -31848,16 +31848,16 @@
         <v>989</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="F55" s="181" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>725</v>
@@ -31887,16 +31887,16 @@
         <v>989</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="F56" s="181" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>725</v>
@@ -31923,7 +31923,7 @@
         <v>-23.5</v>
       </c>
       <c r="Y56" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="AE56" s="3">
         <v>0.873</v>
@@ -31937,16 +31937,16 @@
         <v>989</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="F57" s="181" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>725</v>

</xml_diff>